<commit_message>
Changes to ReadMe.md and requirements.txt
</commit_message>
<xml_diff>
--- a/data_voorbeeld/dev2.xlsx
+++ b/data_voorbeeld/dev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RubenVijverman\PycharmProjects\xls2xml\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RubenVijverman\PycharmProjects\xls2xml\data_voorbeeld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC78FD9-670D-4CF9-9FDF-86693DA39F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD034035-62CD-4F0C-82C6-2E0FE598E5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opdracht" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="751">
   <si>
     <t>naam</t>
   </si>
@@ -2289,6 +2289,9 @@
   </si>
   <si>
     <t>test_xls2xml_v2_1</t>
+  </si>
+  <si>
+    <t>pompfilter</t>
   </si>
 </sst>
 </file>
@@ -2725,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2787,7 +2790,7 @@
     <col min="55" max="55" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3039,7 +3042,7 @@
       <c r="BB2" s="7"/>
       <c r="BC2" s="7"/>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
@@ -3134,7 +3137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" hidden="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3470,17 +3473,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="K2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="W3:Z3"/>
     <mergeCell ref="AW3:AX3"/>
     <mergeCell ref="AY3:AZ3"/>
     <mergeCell ref="AV2:BC2"/>
@@ -3490,6 +3482,17 @@
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AO2:AU2"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="K3:N3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
@@ -3505,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:DD9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3620,7 +3623,7 @@
     <col min="108" max="108" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -4092,7 +4095,7 @@
       <c r="DC2" s="7"/>
       <c r="DD2" s="7"/>
     </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
@@ -4249,7 +4252,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="I4" s="1" t="s">
         <v>97</v>
       </c>
@@ -4416,7 +4419,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="M5" s="6" t="s">
         <v>9</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="M6" s="1" t="s">
         <v>0</v>
       </c>
@@ -4596,7 +4599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:108" hidden="1" x14ac:dyDescent="0.3">
       <c r="N7" s="1" t="s">
         <v>3</v>
       </c>
@@ -5012,27 +5015,17 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="M4:U4"/>
-    <mergeCell ref="I3:U3"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="AE5:AI5"/>
-    <mergeCell ref="AA4:AI4"/>
-    <mergeCell ref="X3:AJ3"/>
-    <mergeCell ref="AO6:AQ6"/>
-    <mergeCell ref="AN5:AQ5"/>
-    <mergeCell ref="AR5:AV5"/>
-    <mergeCell ref="AN4:AV4"/>
-    <mergeCell ref="AK3:AW3"/>
-    <mergeCell ref="BB6:BD6"/>
-    <mergeCell ref="BA5:BD5"/>
-    <mergeCell ref="BE5:BI5"/>
-    <mergeCell ref="BA4:BI4"/>
-    <mergeCell ref="AX3:BJ3"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="CO3:CS3"/>
+    <mergeCell ref="CN2:CT2"/>
+    <mergeCell ref="CX3:CY3"/>
+    <mergeCell ref="CZ3:DA3"/>
+    <mergeCell ref="CW2:DD2"/>
+    <mergeCell ref="CB3:CD3"/>
+    <mergeCell ref="CF3:CG3"/>
+    <mergeCell ref="CH3:CI3"/>
+    <mergeCell ref="CJ3:CK3"/>
+    <mergeCell ref="CA2:CK2"/>
     <mergeCell ref="BK3:BL3"/>
     <mergeCell ref="I2:BL2"/>
     <mergeCell ref="BR5:BT5"/>
@@ -5040,17 +5033,27 @@
     <mergeCell ref="BU4:BY4"/>
     <mergeCell ref="BQ3:BY3"/>
     <mergeCell ref="BP2:BZ2"/>
-    <mergeCell ref="CB3:CD3"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CH3:CI3"/>
-    <mergeCell ref="CJ3:CK3"/>
-    <mergeCell ref="CA2:CK2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="CO3:CS3"/>
-    <mergeCell ref="CN2:CT2"/>
-    <mergeCell ref="CX3:CY3"/>
-    <mergeCell ref="CZ3:DA3"/>
-    <mergeCell ref="CW2:DD2"/>
+    <mergeCell ref="BB6:BD6"/>
+    <mergeCell ref="BA5:BD5"/>
+    <mergeCell ref="BE5:BI5"/>
+    <mergeCell ref="BA4:BI4"/>
+    <mergeCell ref="AX3:BJ3"/>
+    <mergeCell ref="AO6:AQ6"/>
+    <mergeCell ref="AN5:AQ5"/>
+    <mergeCell ref="AR5:AV5"/>
+    <mergeCell ref="AN4:AV4"/>
+    <mergeCell ref="AK3:AW3"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="AA4:AI4"/>
+    <mergeCell ref="X3:AJ3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="M4:U4"/>
+    <mergeCell ref="I3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B1000001" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -5086,8 +5089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BB7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5148,7 +5151,7 @@
     <col min="54" max="54" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -5312,7 +5315,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -5404,7 +5407,7 @@
       <c r="BA2" s="7"/>
       <c r="BB2" s="7"/>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" hidden="1" x14ac:dyDescent="0.3">
       <c r="D3"/>
       <c r="F3" s="1" t="s">
         <v>215</v>
@@ -5509,7 +5512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" hidden="1" x14ac:dyDescent="0.3">
       <c r="D4"/>
       <c r="F4"/>
       <c r="V4" s="1" t="s">
@@ -5777,7 +5780,7 @@
         <v>721</v>
       </c>
       <c r="B7" t="s">
-        <v>725</v>
+        <v>750</v>
       </c>
       <c r="C7" t="s">
         <v>749</v>
@@ -5806,12 +5809,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="R2:Z2"/>
-    <mergeCell ref="AA3:AF3"/>
-    <mergeCell ref="AA2:AF2"/>
     <mergeCell ref="AX3:AY3"/>
     <mergeCell ref="AU2:BB2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -5819,6 +5816,12 @@
     <mergeCell ref="AM3:AQ3"/>
     <mergeCell ref="AL2:AR2"/>
     <mergeCell ref="AV3:AW3"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="R2:Z2"/>
+    <mergeCell ref="AA3:AF3"/>
+    <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B1000001" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -5864,8 +5867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:GI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6062,7 +6065,7 @@
     <col min="191" max="191" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>212</v>
       </c>
@@ -6637,7 +6640,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>212</v>
       </c>
@@ -6844,7 +6847,7 @@
       <c r="GH2" s="7"/>
       <c r="GI2" s="7"/>
     </row>
-    <row r="3" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>90</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="H4" s="1" t="s">
         <v>64</v>
       </c>
@@ -7424,7 +7427,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="5" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
@@ -7653,7 +7656,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="AF6" s="1" t="s">
         <v>0</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="CG7" s="1" t="s">
         <v>0</v>
       </c>
@@ -7876,7 +7879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:191" hidden="1" x14ac:dyDescent="0.3">
       <c r="CH8" s="1" t="s">
         <v>3</v>
       </c>
@@ -9407,23 +9410,29 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V4:Z4"/>
-    <mergeCell ref="BI4:BM4"/>
-    <mergeCell ref="BS5:BW5"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BB3:BX3"/>
-    <mergeCell ref="O2:BX2"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AE4:AK4"/>
-    <mergeCell ref="O3:AK3"/>
-    <mergeCell ref="AO4:AS4"/>
-    <mergeCell ref="AV5:AZ5"/>
-    <mergeCell ref="AU4:BA4"/>
-    <mergeCell ref="AL3:BA3"/>
+    <mergeCell ref="GD2:GI2"/>
+    <mergeCell ref="FO5:FP5"/>
+    <mergeCell ref="FN4:FQ4"/>
+    <mergeCell ref="FS5:FW5"/>
+    <mergeCell ref="FR4:FX4"/>
+    <mergeCell ref="FZ4:GA4"/>
+    <mergeCell ref="EQ4:ER4"/>
+    <mergeCell ref="ES4:ET4"/>
+    <mergeCell ref="EP3:EW3"/>
+    <mergeCell ref="EY4:EZ4"/>
+    <mergeCell ref="FJ4:FM4"/>
+    <mergeCell ref="EX3:GC3"/>
+    <mergeCell ref="EB5:EF5"/>
+    <mergeCell ref="DS4:EF4"/>
+    <mergeCell ref="DS3:EH3"/>
+    <mergeCell ref="EJ4:EN4"/>
+    <mergeCell ref="EI3:EO3"/>
+    <mergeCell ref="DS5:EA5"/>
+    <mergeCell ref="DD7:DF7"/>
+    <mergeCell ref="DC6:DF6"/>
+    <mergeCell ref="DG6:DK6"/>
+    <mergeCell ref="DC5:DK5"/>
+    <mergeCell ref="DL5:DP5"/>
     <mergeCell ref="BY2:CB2"/>
     <mergeCell ref="CH7:CJ7"/>
     <mergeCell ref="CG6:CJ6"/>
@@ -9440,29 +9449,23 @@
     <mergeCell ref="DT7:DV7"/>
     <mergeCell ref="DS6:DV6"/>
     <mergeCell ref="DW6:EA6"/>
-    <mergeCell ref="DS5:EA5"/>
-    <mergeCell ref="DD7:DF7"/>
-    <mergeCell ref="DC6:DF6"/>
-    <mergeCell ref="DG6:DK6"/>
-    <mergeCell ref="DC5:DK5"/>
-    <mergeCell ref="DL5:DP5"/>
-    <mergeCell ref="EB5:EF5"/>
-    <mergeCell ref="DS4:EF4"/>
-    <mergeCell ref="DS3:EH3"/>
-    <mergeCell ref="EJ4:EN4"/>
-    <mergeCell ref="EI3:EO3"/>
-    <mergeCell ref="EQ4:ER4"/>
-    <mergeCell ref="ES4:ET4"/>
-    <mergeCell ref="EP3:EW3"/>
-    <mergeCell ref="EY4:EZ4"/>
-    <mergeCell ref="FJ4:FM4"/>
-    <mergeCell ref="EX3:GC3"/>
-    <mergeCell ref="GD2:GI2"/>
-    <mergeCell ref="FO5:FP5"/>
-    <mergeCell ref="FN4:FQ4"/>
-    <mergeCell ref="FS5:FW5"/>
-    <mergeCell ref="FR4:FX4"/>
-    <mergeCell ref="FZ4:GA4"/>
+    <mergeCell ref="BI4:BM4"/>
+    <mergeCell ref="BS5:BW5"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BB3:BX3"/>
+    <mergeCell ref="O2:BX2"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AE4:AK4"/>
+    <mergeCell ref="O3:AK3"/>
+    <mergeCell ref="AO4:AS4"/>
+    <mergeCell ref="AV5:AZ5"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="AL3:BA3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V4:Z4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="11">
@@ -11021,26 +11024,21 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="I5:Q5"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="U5:AC5"/>
-    <mergeCell ref="R4:AD4"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AM6:AQ6"/>
-    <mergeCell ref="AI5:AQ5"/>
-    <mergeCell ref="AE4:AQ4"/>
-    <mergeCell ref="AV7:AX7"/>
-    <mergeCell ref="AU6:AX6"/>
-    <mergeCell ref="AY6:BC6"/>
-    <mergeCell ref="AU5:BC5"/>
-    <mergeCell ref="AR4:BD4"/>
+    <mergeCell ref="CW3:DA3"/>
+    <mergeCell ref="CV2:DB2"/>
+    <mergeCell ref="DE3:DF3"/>
+    <mergeCell ref="DG3:DH3"/>
+    <mergeCell ref="DD2:DK2"/>
+    <mergeCell ref="CN5:CP5"/>
+    <mergeCell ref="CM4:CP4"/>
+    <mergeCell ref="CQ4:CU4"/>
+    <mergeCell ref="CM3:CU3"/>
+    <mergeCell ref="CH2:CU2"/>
+    <mergeCell ref="CA4:CE4"/>
+    <mergeCell ref="BW3:CE3"/>
+    <mergeCell ref="BR2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH3:CL3"/>
     <mergeCell ref="E2:BJ2"/>
     <mergeCell ref="BK2:BL2"/>
     <mergeCell ref="BO2:BP2"/>
@@ -11049,21 +11047,26 @@
     <mergeCell ref="BW4:BZ4"/>
     <mergeCell ref="E3:AD3"/>
     <mergeCell ref="AE3:BD3"/>
-    <mergeCell ref="CA4:CE4"/>
-    <mergeCell ref="BW3:CE3"/>
-    <mergeCell ref="BR2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH3:CL3"/>
-    <mergeCell ref="CN5:CP5"/>
-    <mergeCell ref="CM4:CP4"/>
-    <mergeCell ref="CQ4:CU4"/>
-    <mergeCell ref="CM3:CU3"/>
-    <mergeCell ref="CH2:CU2"/>
-    <mergeCell ref="CW3:DA3"/>
-    <mergeCell ref="CV2:DB2"/>
-    <mergeCell ref="DE3:DF3"/>
-    <mergeCell ref="DG3:DH3"/>
-    <mergeCell ref="DD2:DK2"/>
+    <mergeCell ref="AV7:AX7"/>
+    <mergeCell ref="AU6:AX6"/>
+    <mergeCell ref="AY6:BC6"/>
+    <mergeCell ref="AU5:BC5"/>
+    <mergeCell ref="AR4:BD4"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AM6:AQ6"/>
+    <mergeCell ref="AI5:AQ5"/>
+    <mergeCell ref="AE4:AQ4"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="U5:AC5"/>
+    <mergeCell ref="R4:AD4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="I5:Q5"/>
+    <mergeCell ref="E4:Q4"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B1000001" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11791,17 +11794,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="L2:T2"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="Z4:AH4"/>
     <mergeCell ref="AY3:AZ3"/>
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="AX2:BE2"/>
@@ -11810,6 +11802,17 @@
     <mergeCell ref="Z2:AN2"/>
     <mergeCell ref="AQ3:AU3"/>
     <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="Z4:AH4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1000001" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -12735,11 +12738,14 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="AH2:AU2"/>
+    <mergeCell ref="BD2:BG2"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BH2:BK2"/>
+    <mergeCell ref="BM3:BQ3"/>
+    <mergeCell ref="BL2:BR2"/>
+    <mergeCell ref="AH3:AL3"/>
     <mergeCell ref="AN5:AP5"/>
     <mergeCell ref="AM4:AP4"/>
     <mergeCell ref="AQ4:AU4"/>
@@ -12752,14 +12758,11 @@
     <mergeCell ref="X4:AE4"/>
     <mergeCell ref="V3:AG3"/>
     <mergeCell ref="S2:AG2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="AH2:AU2"/>
-    <mergeCell ref="BD2:BG2"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BH2:BK2"/>
-    <mergeCell ref="BM3:BQ3"/>
-    <mergeCell ref="BL2:BR2"/>
-    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="B2:L2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E1000001 J9:J1000001" xr:uid="{00000000-0002-0000-0600-000000000000}">

</xml_diff>